<commit_message>
finalização do min-max e drive do inventário
</commit_message>
<xml_diff>
--- a/Listagens de Inventário/FILIAL TATUAPE-SP 1337 - LAB - DESCARTÁVEIS TATUAPÉ.xlsx
+++ b/Listagens de Inventário/FILIAL TATUAPE-SP 1337 - LAB - DESCARTÁVEIS TATUAPÉ.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4695</v>
+        <v>5017</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4694</v>
+        <v>5016</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4687</v>
+        <v>5006</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4757</v>
+        <v>5080</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4758</v>
+        <v>5083</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4738</v>
+        <v>5057</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4763</v>
+        <v>5088</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4762</v>
+        <v>5087</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4764</v>
+        <v>5089</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -849,7 +849,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4765</v>
+        <v>5090</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4700</v>
+        <v>5048</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -905,7 +905,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>221134L</t>
+          <t>C221134L</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -927,16 +927,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4766</v>
+        <v>5021</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>10023889</t>
+          <t>10022814</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>BAG TARJA VERDE 20 X 40</t>
+          <t>TUBO HEPARINA TRACE (AMETAL) 6ML</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -944,7 +944,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>221134L</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
@@ -964,16 +968,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4814</v>
+        <v>5091</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10024053</t>
+          <t>10023889</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>KIT PCR (BAG TARJA ROXA P - SWAB RAYON - PANFLETO - TUBO TRACE)</t>
+          <t>BAG TARJA VERDE 20 X 40</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1001,16 +1005,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4730</v>
+        <v>5142</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>10024098</t>
+          <t>10024053</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>TUBO DE CITRATO DE SODIO 2ML</t>
+          <t>KIT PCR (BAG TARJA ROXA P - SWAB RAYON - PANFLETO - TUBO TRACE)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1018,11 +1022,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>C23033NV</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4745</v>
+        <v>5052</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>C2306389</t>
+          <t>C23033NV</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -1083,16 +1083,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4729</v>
+        <v>5064</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>10024454</t>
+          <t>10024098</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>TUBO HEPARINA 4ML</t>
+          <t>TUBO DE CITRATO DE SODIO 2ML</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>C2303343</t>
+          <t>C2306389</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1124,16 +1124,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4674</v>
+        <v>5050</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>10024485</t>
+          <t>10024454</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>SALIVETE</t>
+          <t>TUBO HEPARINA 4ML</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1093621</t>
+          <t>C230233Y</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1165,16 +1165,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4678</v>
+        <v>4993</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10024644</t>
+          <t>10024485</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>COLETOR DE FEZES SECO</t>
+          <t>SALIVETE</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12300170</t>
+          <t>1093621</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1206,16 +1206,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4668</v>
+        <v>4998</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10024645</t>
+          <t>10024644</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>RECIPIENTE URINA 24H</t>
+          <t>COLETOR DE FEZES SECO</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0323P16</t>
+          <t>12300359</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4669</v>
+        <v>4986</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1288,16 +1288,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4749</v>
+        <v>4987</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10024648</t>
+          <t>10024645</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>TUBO EAS ESTERIL 80ML</t>
+          <t>RECIPIENTE URINA 24H</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1307,7 +1307,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>CE040822A</t>
+          <t>0923P18</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1329,16 +1329,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4767</v>
+        <v>5070</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>10024649</t>
+          <t>10024648</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>BAG TARJA ROXA 13 X 24</t>
+          <t>TUBO EAS ESTERIL 80ML</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1346,7 +1346,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>CE190423M</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
@@ -1366,16 +1370,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4768</v>
+        <v>5092</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10024655</t>
+          <t>10024649</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>BAG TARJA VERMELHA 20 X 40</t>
+          <t>BAG TARJA ROXA 13 X 24</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1403,16 +1407,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4712</v>
+        <v>5093</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>10024656</t>
+          <t>10024655</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>KIT ACIDO 0,8 ML/L 20 ML</t>
+          <t>BAG TARJA VERMELHA 20 X 40</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1420,11 +1424,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>258110</t>
-        </is>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
@@ -1444,16 +1444,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4752</v>
+        <v>5035</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10024658</t>
+          <t>10024656</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">KIT URINA 12ML FRASCO - TUBO </t>
+          <t>KIT ACIDO 0,8 ML/L 20 ML</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>KE270723B</t>
+          <t>258110</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1485,108 +1485,112 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4690</v>
+        <v>5075</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>10024658</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KIT URINA 12ML FRASCO - TUBO </t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>KE021023C</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>5007</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>10024659</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t xml:space="preserve">LAMINA PAPANICOLAU FOSCA
 </t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>202201</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>UNIDADE</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>FILIAL TATUAPE-SP 1337</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>4688</v>
-      </c>
-      <c r="D28" t="inlineStr">
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>202111</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>10024659</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t xml:space="preserve">LAMINA PAPANICOLAU FOSCA
 </t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>202111</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>UNIDADE</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>FILIAL TATUAPE-SP 1337</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>4769</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>10024663</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>TAMPA PARA TUBO AMBAR 12 X 75</t>
-        </is>
-      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>LAB</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>202201</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
@@ -1606,16 +1610,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>4545</v>
+        <v>5094</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>10024664</t>
+          <t>10024663</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>TUBO AMBAR 12 X 75 CRAL</t>
+          <t>TAMPA PARA TUBO AMBAR 12 X 75</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1623,11 +1627,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>23100305</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4544</v>
+        <v>5022</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>23033003</t>
+          <t>22121403</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -1688,16 +1688,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>4732</v>
+        <v>5028</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>10024706</t>
+          <t>10024664</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>TUBO 2KEDTA 5ML</t>
+          <t>TUBO AMBAR 12 X 75 CRAL</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>C23033SH</t>
+          <t>23100305</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -1729,16 +1729,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4701</v>
+        <v>5027</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>10024706</t>
+          <t>10024664</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>TUBO 2KEDTA 5ML</t>
+          <t>TUBO AMBAR 12 X 75 CRAL</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>22113GM</t>
+          <t>23033003</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -1770,16 +1770,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4821</v>
+        <v>5054</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>10025227</t>
+          <t>10024706</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>SWAB CARY BLAIR</t>
+          <t>TUBO 2KEDTA 5ML</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1787,7 +1787,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>C23033SH</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
@@ -1807,16 +1811,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4714</v>
+        <v>5049</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>10025398</t>
+          <t>10024706</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>TUBO ACIDO BORICO 4ML</t>
+          <t>TUBO 2KEDTA 5ML</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1826,7 +1830,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>3039729</t>
+          <t>C22113BY</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -1848,16 +1852,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4748</v>
+        <v>5141</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>10025433</t>
+          <t>10025227</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>TUBO TRACE SEM ADITIVO 6ML</t>
+          <t>SWAB CARY BLAIR</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1865,11 +1869,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>C230735J</t>
-        </is>
-      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
@@ -1889,16 +1889,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4737</v>
+        <v>5038</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>10025433</t>
+          <t>10025398</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>TUBO TRACE SEM ADITIVO 6ML</t>
+          <t>TUBO ACIDO BORICO 4ML</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>C230533F</t>
+          <t>3039729</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -1930,16 +1930,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4681</v>
+        <v>5069</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>10025504</t>
+          <t>10025433</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>ETIQUETA TERMICA 50X25 - 1 COLUNA - TARJA VERDE</t>
+          <t>TUBO TRACE SEM ADITIVO 6ML</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>15675</t>
+          <t>C230735J</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
@@ -1971,16 +1971,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4682</v>
+        <v>5056</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>10025504</t>
+          <t>10025433</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>ETIQUETA TERMICA 50X25 - 1 COLUNA - TARJA VERDE</t>
+          <t>TUBO TRACE SEM ADITIVO 6ML</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>15912</t>
+          <t>C230533F</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -2012,16 +2012,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4818</v>
+        <v>5001</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>10027308</t>
+          <t>10025504</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>SWAB CARVAO</t>
+          <t>ETIQUETA TERMICA 50X25 - 1 COLUNA - TARJA VERDE</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2029,7 +2029,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>16232</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
@@ -2049,16 +2053,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>4770</v>
+        <v>5143</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>10027318</t>
+          <t>10027308</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>BAG TARJA ROXA 18 X 22</t>
+          <t>SWAB CARVAO</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2086,16 +2090,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>4683</v>
+        <v>5095</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>10027355</t>
+          <t>10027318</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>PAPEL FILTRO PEZINHO</t>
+          <t>BAG TARJA ROXA 18 X 22</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2103,11 +2107,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>17426732</t>
-        </is>
-      </c>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>4684</v>
+        <v>5002</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>17529598</t>
+          <t>17426732</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -2168,16 +2168,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4727</v>
+        <v>5003</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>10028676</t>
+          <t>10027355</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>TUBO DE CITRATO DE SODIO 4ML</t>
+          <t>PAPEL FILTRO PEZINHO</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>C2302347</t>
+          <t>17529598</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -2209,7 +2209,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4726</v>
+        <v>5051</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>C221234Q</t>
+          <t>C2302347</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>4746</v>
+        <v>5067</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2291,7 +2291,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4731</v>
+        <v>5053</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4728</v>
+        <v>5065</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>C230239P</t>
+          <t>C2307348</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -2373,16 +2373,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4721</v>
+        <v>5066</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>10028678</t>
+          <t>10028677</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>TUBO FLUORETO DE SODIO 2ML</t>
+          <t>TUBO TRANSPORTE 4ML</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>A221039T</t>
+          <t>C230734A</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -2414,7 +2414,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4722</v>
+        <v>5045</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -2455,16 +2455,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4735</v>
+        <v>5044</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>10028679</t>
+          <t>10028678</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>TUBO SORO GEL 5ML</t>
+          <t>TUBO FLUORETO DE SODIO 2ML</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>C23043G9</t>
+          <t>A221039T</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
@@ -2496,7 +2496,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4734</v>
+        <v>5055</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>C23043G8</t>
+          <t>C23043QR</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -2537,7 +2537,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4736</v>
+        <v>5061</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>C23043GA</t>
+          <t>C230535D</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -2578,7 +2578,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4742</v>
+        <v>5060</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>C230535D</t>
+          <t>C230535B</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
@@ -2619,16 +2619,16 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4741</v>
+        <v>5068</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>10028679</t>
+          <t>10028680</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>TUBO SORO GEL 5ML</t>
+          <t>TUBO K3EDTA 4ML</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>C230535B</t>
+          <t>C230734R</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>4733</v>
+        <v>5063</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>C230434A</t>
+          <t>C230633D</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -2701,7 +2701,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4739</v>
+        <v>5058</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4740</v>
+        <v>5062</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>C230534P</t>
+          <t>C2306339</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2783,7 +2783,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4743</v>
+        <v>5059</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>C2306339</t>
+          <t>C230534P</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -2824,16 +2824,16 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>4744</v>
+        <v>5140</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>10028680</t>
+          <t>10028681</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>TUBO K3EDTA 4ML</t>
+          <t>TUBO HEPARINA 9ML</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2841,11 +2841,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>C230633D</t>
-        </is>
-      </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
@@ -2865,16 +2861,16 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4747</v>
+        <v>4990</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>10028680</t>
+          <t>10029309</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>TUBO K3EDTA 4ML</t>
+          <t>PORTA LAMINA DE CITOLOGIA</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2884,7 +2880,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>C230734R</t>
+          <t>104143</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -2906,16 +2902,16 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>4817</v>
+        <v>4989</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>10028681</t>
+          <t>10029309</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>TUBO HEPARINA 9ML</t>
+          <t>PORTA LAMINA DE CITOLOGIA</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2923,7 +2919,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>103448</t>
+        </is>
+      </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr">
         <is>
@@ -2943,16 +2943,17 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4671</v>
+        <v>5128</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>10029309</t>
+          <t>10029753</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>PORTA LAMINA DE CITOLOGIA</t>
+          <t xml:space="preserve">BAG TOXICOLOGICO 13 X 24 LARANJA 
+</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2960,11 +2961,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>103448</t>
-        </is>
-      </c>
+      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
@@ -2984,16 +2981,16 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>4802</v>
+        <v>5129</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>10029753</t>
+          <t>10029754</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">BAG TOXICOLOGICO 13 X 24 LARANJA 
+          <t xml:space="preserve">BAG TOXICOLOGICO 30 X 43 LARANJA 
 </t>
         </is>
       </c>
@@ -3022,17 +3019,16 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>4803</v>
+        <v>5000</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>10029754</t>
+          <t>10030001</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">BAG TOXICOLOGICO 30 X 43 LARANJA 
-</t>
+          <t>ADAPTADOR PARA COLETA A VACUO TRANSPARENTE - CANHAO</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3040,7 +3036,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>1306346</t>
+        </is>
+      </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr">
         <is>
@@ -3060,7 +3060,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>4680</v>
+        <v>5039</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>1306346</t>
+          <t>3142490</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -3101,16 +3101,16 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4715</v>
+        <v>5037</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>10030001</t>
+          <t>10030003</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>ADAPTADOR PARA COLETA A VACUO TRANSPARENTE - CANHAO</t>
+          <t>AGULHA A VACUO 21G COM TRAVAS DE SEGURANCA (VERDE)</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>3142490</t>
+          <t>3026491</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -3142,16 +3142,16 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4816</v>
+        <v>4992</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>10030003</t>
+          <t>10030004</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>AGULHA A VACUO 21G COM TRAVAS DE SEGURANCA (VERDE)</t>
+          <t>AGULHA A VACUO 22G COM TRAVAS DE SEGURANCA (PRETA)</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3159,7 +3159,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>1091824</t>
+        </is>
+      </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
         <is>
@@ -3179,16 +3183,16 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>4673</v>
+        <v>4983</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>10030004</t>
+          <t>10030016</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>AGULHA A VACUO 22G COM TRAVAS DE SEGURANCA (PRETA)</t>
+          <t>ALCOOL 70% LÍQUIDO</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3198,13 +3202,13 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>1091824</t>
+          <t>001523A</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
+          <t>LITRO</t>
         </is>
       </c>
     </row>
@@ -3220,16 +3224,16 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>4664</v>
+        <v>4997</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>10030016</t>
+          <t>10030017</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>ALCOOL 70% LÍQUIDO</t>
+          <t>ALGODAO HIDROFILO</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3239,13 +3243,13 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>001523A</t>
+          <t>1222</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr">
         <is>
-          <t>LITRO</t>
+          <t>UNIDADE</t>
         </is>
       </c>
     </row>
@@ -3261,16 +3265,16 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4667</v>
+        <v>5102</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>10030017</t>
+          <t>10030019</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>ALGODAO HIDROFILO</t>
+          <t>AVENTAL DESCARTAVEL</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3278,11 +3282,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>0222</t>
-        </is>
-      </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr">
         <is>
@@ -3302,16 +3302,16 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>4777</v>
+        <v>5103</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>10030019</t>
+          <t>10030020</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>AVENTAL DESCARTAVEL</t>
+          <t>BOBINA PLASTICA PICOTADA 30X40 (3L)</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3339,16 +3339,16 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>4778</v>
+        <v>4988</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>10030020</t>
+          <t>10030021</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>BOBINA PLASTICA PICOTADA 30X40 (3L)</t>
+          <t>BOLSA DE GEL PROMOCIONAL</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3356,7 +3356,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>100K</t>
+        </is>
+      </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr">
         <is>
@@ -3376,16 +3380,16 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>4670</v>
+        <v>5071</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>10030021</t>
+          <t>10030026</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>BOLSA DE GEL PROMOCIONAL</t>
+          <t>CAIXA COLETORA DE PERFURO CORTANTE 1,5L</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3395,7 +3399,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>100K</t>
+          <t>CO15AA0182</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -3417,16 +3421,16 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4724</v>
+        <v>5047</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>10030026</t>
+          <t>10030028</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>CAIXA COLETORA DE PERFURO CORTANTE 1,5L</t>
+          <t>CAMPO CIRURGICO DESCARTAVEL 0,45X0,45 (TNT)</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3436,7 +3440,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>C015AA0179</t>
+          <t>C1943</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -3458,16 +3462,16 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4717</v>
+        <v>5034</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>10030028</t>
+          <t>10030030</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>CAMPO CIRURGICO DESCARTAVEL 0,45X0,45 (TNT)</t>
+          <t>CURATIVO REDONDO PERSONALIZADO BEEP</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3477,7 +3481,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>48920</t>
+          <t>24723</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -3499,16 +3503,16 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>4725</v>
+        <v>5004</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>10030028</t>
+          <t>10030030</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>CAMPO CIRURGICO DESCARTAVEL 0,45X0,45 (TNT)</t>
+          <t>CURATIVO REDONDO PERSONALIZADO BEEP</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3518,7 +3522,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>C1943</t>
+          <t>18023</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
@@ -3540,16 +3544,16 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>4685</v>
+        <v>5043</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>10030030</t>
+          <t>10030034</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>CURATIVO REDONDO PERSONALIZADO BEEP</t>
+          <t>GAZE HIDROFILA ESTERIL</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3559,7 +3563,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>18023</t>
+          <t>A17-1</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -3581,16 +3585,16 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4711</v>
+        <v>5046</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>10030030</t>
+          <t>10030034</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>CURATIVO REDONDO PERSONALIZADO BEEP</t>
+          <t>GAZE HIDROFILA ESTERIL</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3600,7 +3604,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>24723</t>
+          <t>B29-1</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
@@ -3622,7 +3626,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>4692</v>
+        <v>5014</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -3663,16 +3667,16 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4720</v>
+        <v>5076</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>10030034</t>
+          <t>10030035</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>GAZE HIDROFILA ESTERIL</t>
+          <t>HIPOCLORITO 1%</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3682,13 +3686,13 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>A17-1</t>
+          <t>P23080016</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
+          <t>LITRO</t>
         </is>
       </c>
     </row>
@@ -3704,16 +3708,16 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>4723</v>
+        <v>5100</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>10030034</t>
+          <t>10030036</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>GAZE HIDROFILA ESTERIL</t>
+          <t>KIT SEXAGEM - BALAO VERDE BEEP</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3721,11 +3725,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>B29-1</t>
-        </is>
-      </c>
+      <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr">
         <is>
@@ -3745,16 +3745,16 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4753</v>
+        <v>5101</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>10030035</t>
+          <t>10030037</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>HIPOCLORITO 1%</t>
+          <t>KIT SEXAGEM - CARTAO KIT SEXAGEM</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3762,15 +3762,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>P23080016</t>
-        </is>
-      </c>
+      <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr">
         <is>
-          <t>LITRO</t>
+          <t>UNIDADE</t>
         </is>
       </c>
     </row>
@@ -3786,16 +3782,16 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>4775</v>
+        <v>5104</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>10030036</t>
+          <t>10030038</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - BALAO VERDE BEEP</t>
+          <t>KIT SEXAGEM - EMBALAGEM BASCULANTE</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3823,16 +3819,16 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>4776</v>
+        <v>5146</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>10030037</t>
+          <t>10030039</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - CARTAO KIT SEXAGEM</t>
+          <t>KIT SEXAGEM - FITA CETIM (BRANCA 10M X 16MM)</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3860,16 +3856,16 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4779</v>
+        <v>5147</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>10030038</t>
+          <t>10030040</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - EMBALAGEM BASCULANTE</t>
+          <t>KIT SEXAGEM - FITA CETIM (BRANCA 60M X 16MM)</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3897,16 +3893,16 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4823</v>
+        <v>5085</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>10030039</t>
+          <t>10030041</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - FITA CETIM (BRANCA 10M X 16MM)</t>
+          <t>KIT SEXAGEM - PAPEL PICADO CINTILANTE AZUL</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3918,7 +3914,7 @@
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
+          <t>QUILOGRAMA</t>
         </is>
       </c>
     </row>
@@ -3934,16 +3930,16 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4815</v>
+        <v>5086</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>10030040</t>
+          <t>10030042</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - FITA CETIM (BRANCA 60M X 16MM)</t>
+          <t>KIT SEXAGEM - PAPEL PICADO CINTILANTE ROSA</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3955,7 +3951,7 @@
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
+          <t>QUILOGRAMA</t>
         </is>
       </c>
     </row>
@@ -3971,16 +3967,16 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>4760</v>
+        <v>5042</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>10030041</t>
+          <t>10030044</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - PAPEL PICADO CINTILANTE AZUL</t>
+          <t>LANCETA BD 2,50X1,00</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3988,11 +3984,15 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>92779997</t>
+        </is>
+      </c>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr">
         <is>
-          <t>QUILOGRAMA</t>
+          <t>UNIDADE</t>
         </is>
       </c>
     </row>
@@ -4008,16 +4008,16 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4761</v>
+        <v>5079</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>10030042</t>
+          <t>10030045</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>KIT SEXAGEM - PAPEL PICADO CINTILANTE ROSA</t>
+          <t>LUVA NITRÍLICA SEM PO G</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -4025,11 +4025,15 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>SNFTAA073L</t>
+        </is>
+      </c>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr">
         <is>
-          <t>QUILOGRAMA</t>
+          <t>UNIDADE</t>
         </is>
       </c>
     </row>
@@ -4045,16 +4049,16 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4719</v>
+        <v>5025</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>10030044</t>
+          <t>10030046</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>LANCETA BD 2,50X1,00</t>
+          <t>LUVA NITRÍLICA SEM PO M</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4064,7 +4068,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>9277997</t>
+          <t>230204187</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
@@ -4086,16 +4090,16 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4756</v>
+        <v>5081</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>10030045</t>
+          <t>10030046</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>LUVA NITRÍLICA SEM PO G</t>
+          <t>LUVA NITRÍLICA SEM PO M</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4105,7 +4109,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>SNFTAA073L</t>
+          <t>XL221222</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -4127,7 +4131,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4703</v>
+        <v>5072</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -4146,7 +4150,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>230100426</t>
+          <t>IN22014699</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
@@ -4168,7 +4172,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>4750</v>
+        <v>5073</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -4209,16 +4213,16 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>4706</v>
+        <v>5074</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>10030046</t>
+          <t>10030047</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>LUVA NITRÍLICA SEM PO M</t>
+          <t>LUVA NITRÍLICA SEM PO P</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -4228,7 +4232,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>230204187</t>
+          <t>IN22016733</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -4250,7 +4254,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4705</v>
+        <v>5011</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -4269,7 +4273,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>230204184</t>
+          <t>20230044A</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -4291,7 +4295,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4707</v>
+        <v>5023</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -4310,7 +4314,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>230302443</t>
+          <t>23000783</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
@@ -4332,7 +4336,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>4751</v>
+        <v>5026</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -4351,7 +4355,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>IN22016733</t>
+          <t>230302443</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
@@ -4373,16 +4377,16 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>4755</v>
+        <v>5082</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>10030048</t>
+          <t>10030047</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>LUVA NITRÍLICA SEM PO PP</t>
+          <t>LUVA NITRÍLICA SEM PO P</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -4392,7 +4396,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>SNFTAA065X</t>
+          <t>Z2889022J</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -4414,16 +4418,16 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4696</v>
+        <v>5078</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>10030050</t>
+          <t>10030048</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>MASCARA CIRURGICA TRIPLA DESCARTAVEL</t>
+          <t>LUVA NITRÍLICA SEM PO PP</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -4433,7 +4437,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>22008103</t>
+          <t>SNFTAA065X</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -4455,7 +4459,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>4697</v>
+        <v>5018</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -4474,7 +4478,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>22014504</t>
+          <t>22008103</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -4496,7 +4500,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>4698</v>
+        <v>5019</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -4515,7 +4519,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>22015405</t>
+          <t>22014504</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
@@ -4537,16 +4541,16 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>4718</v>
+        <v>5009</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>10030051</t>
+          <t>10030050</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>MASCARA DESCARTAVEL N95</t>
+          <t>MASCARA CIRURGICA TRIPLA DESCARTAVEL</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -4556,7 +4560,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>5041747</t>
+          <t>20220017</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -4578,16 +4582,16 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>4754</v>
+        <v>5036</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>10030051</t>
+          <t>10030050</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>MASCARA DESCARTAVEL N95</t>
+          <t>MASCARA CIRURGICA TRIPLA DESCARTAVEL</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4597,7 +4601,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>SMNDAA0011</t>
+          <t>2MEFAA0006</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
@@ -4619,16 +4623,16 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>4771</v>
+        <v>5041</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>10030053</t>
+          <t>10030051</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>PAPEL ALUMÍNIO</t>
+          <t>MASCARA DESCARTAVEL N95</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4636,7 +4640,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>5041747</t>
+        </is>
+      </c>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr">
         <is>
@@ -4656,16 +4664,16 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>4772</v>
+        <v>5077</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>10030054</t>
+          <t>10030051</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>PAPEL TOALHA INTERFOLHADO</t>
+          <t>MASCARA DESCARTAVEL N95</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4673,7 +4681,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>SMNDAA0011</t>
+        </is>
+      </c>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr">
         <is>
@@ -4693,16 +4705,16 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4666</v>
+        <v>5096</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>10030055</t>
+          <t>10030053</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>PONTEIRA UNIVERSAL SEM FILTRO 1.000 µL</t>
+          <t>PAPEL ALUMÍNIO</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4710,11 +4722,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>02/2022</t>
-        </is>
-      </c>
+      <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr">
         <is>
@@ -4734,16 +4742,16 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>4689</v>
+        <v>5097</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>10030056</t>
+          <t>10030054</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>PONTEIRA UNIVERSAL SEM FILTRO 200 µL</t>
+          <t>PAPEL TOALHA INTERFOLHADO</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4751,11 +4759,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2022001</t>
-        </is>
-      </c>
+      <c r="G108" t="inlineStr"/>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr">
         <is>
@@ -4775,16 +4779,16 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4665</v>
+        <v>4985</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>10030057</t>
+          <t>10030055</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>RECIPIENTE PARA COLETA DE FEZES COM CONSERVANTE SAF</t>
+          <t>PONTEIRA UNIVERSAL SEM FILTRO 1.000 µL</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4794,7 +4798,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>002142/S</t>
+          <t>02/2022</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -4816,16 +4820,16 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4819</v>
+        <v>5008</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>10030058</t>
+          <t>10030056</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>SABONETE LÍQUIDO</t>
+          <t>PONTEIRA UNIVERSAL SEM FILTRO 200 µL</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4833,11 +4837,15 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>2022001</t>
+        </is>
+      </c>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr">
         <is>
-          <t>LITRO</t>
+          <t>UNIDADE</t>
         </is>
       </c>
     </row>
@@ -4853,16 +4861,16 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>4693</v>
+        <v>4984</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>10030059</t>
+          <t>10030057</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>SACO COLETOR DE URINA ESTERIL INFANTIL</t>
+          <t>RECIPIENTE PARA COLETA DE FEZES COM CONSERVANTE SAF</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4872,7 +4880,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>211210</t>
+          <t>002091/S</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -4894,16 +4902,16 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>4773</v>
+        <v>5145</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>10030062</t>
+          <t>10030058</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>SACO DE LIXO INFECTANTE 30 LITROS</t>
+          <t>SABONETE LÍQUIDO</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -4915,7 +4923,7 @@
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
+          <t>LITRO</t>
         </is>
       </c>
     </row>
@@ -4931,16 +4939,16 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>4774</v>
+        <v>5015</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>10030063</t>
+          <t>10030059</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>SACO PLASTICO 16X21CM COM ADESIVO PONTA (KIT SEXAGEM)</t>
+          <t>SACO COLETOR DE URINA ESTERIL INFANTIL</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -4948,7 +4956,11 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G113" t="inlineStr"/>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>211210</t>
+        </is>
+      </c>
       <c r="H113" t="inlineStr"/>
       <c r="I113" t="inlineStr">
         <is>
@@ -4968,16 +4980,16 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>4716</v>
+        <v>5098</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>10030065</t>
+          <t>10030062</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>SAPATILHA PROPE</t>
+          <t>SACO DE LIXO INFECTANTE 30 LITROS</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -4985,11 +4997,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>408-23</t>
-        </is>
-      </c>
+      <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr">
         <is>
@@ -5009,16 +5017,16 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4677</v>
+        <v>5099</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>10030066</t>
+          <t>10030063</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>SCALP 21G COM TRAVA DE SEGURANCA</t>
+          <t>SACO PLASTICO 16X21CM COM ADESIVO PONTA (KIT SEXAGEM)</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -5026,11 +5034,7 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>1209870</t>
-        </is>
-      </c>
+      <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr">
         <is>
@@ -5050,16 +5054,16 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>4676</v>
+        <v>5040</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>10030067</t>
+          <t>10030065</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>SCALP 23G COM TRAVA DE SEGURANCA</t>
+          <t>SAPATILHA PROPE</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -5069,7 +5073,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>1194947</t>
+          <t>408-23</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -5091,16 +5095,16 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>4679</v>
+        <v>4996</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>10030068</t>
+          <t>10030066</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>SCALP 25G COM TRAVA DE SEGURANCA</t>
+          <t>SCALP 21G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -5110,7 +5114,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>1299843.</t>
+          <t>1209870</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
@@ -5132,16 +5136,16 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>4713</v>
+        <v>4995</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>10030069</t>
+          <t>10030067</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>SCALP A VACUO 21G COM TRAVA DE SEGURANCA</t>
+          <t>SCALP 23G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -5151,7 +5155,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>2K18A1</t>
+          <t>1194947</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
@@ -5173,16 +5177,16 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>4710</v>
+        <v>4999</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>10030069</t>
+          <t>10030068</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>SCALP A VACUO 21G COM TRAVA DE SEGURANCA</t>
+          <t>SCALP 25G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -5192,7 +5196,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>23C30A1</t>
+          <t>1299843.</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
@@ -5214,7 +5218,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4709</v>
+        <v>5032</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -5233,7 +5237,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>23C29A1</t>
+          <t>23D17A2</t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
@@ -5255,16 +5259,16 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>4708</v>
+        <v>5030</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>10030070</t>
+          <t>10030069</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>SCALP A VACUO 23G COM TRAVA DE SEGURANCA</t>
+          <t>SCALP A VACUO 21G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -5274,7 +5278,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>23A10A1</t>
+          <t>23C29A1</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -5296,16 +5300,16 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>4702</v>
+        <v>5012</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>10030070</t>
+          <t>10030069</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>SCALP A VACUO 23G COM TRAVA DE SEGURANCA</t>
+          <t>SCALP A VACUO 21G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -5315,7 +5319,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>22L29B1</t>
+          <t>20230420</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
@@ -5337,16 +5341,16 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>4686</v>
+        <v>5031</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>10030071</t>
+          <t>10030069</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>SCALP A VACUO 25G COM TRAVA DE SEGURANCA</t>
+          <t>SCALP A VACUO 21G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -5356,7 +5360,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>1B07A1</t>
+          <t>23C30A1</t>
         </is>
       </c>
       <c r="H123" t="inlineStr"/>
@@ -5378,16 +5382,16 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>4675</v>
+        <v>5029</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>10030072</t>
+          <t>10030070</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>SERINGA 10 ML LL SEM TRAVA DE SEGURANCA</t>
+          <t>SCALP A VACUO 23G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -5397,7 +5401,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>1132410</t>
+          <t>23A10A1</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
@@ -5419,16 +5423,16 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>4672</v>
+        <v>5033</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>10030075</t>
+          <t>10030070</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>SERINGA 5 ML LL SEM TRAVA DE SEGURANCA</t>
+          <t>SCALP A VACUO 23G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -5438,7 +5442,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>1048024</t>
+          <t>23D19A1</t>
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
@@ -5460,16 +5464,16 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>4704</v>
+        <v>5005</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>10030078</t>
+          <t>10030071</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>SWAB ALCOOL 70°</t>
+          <t>SCALP A VACUO 25G COM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -5479,7 +5483,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>23020106</t>
+          <t>1A20A1</t>
         </is>
       </c>
       <c r="H126" t="inlineStr"/>
@@ -5501,16 +5505,16 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4699</v>
+        <v>4994</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>10030078</t>
+          <t>10030072</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>SWAB ALCOOL 70°</t>
+          <t>SERINGA 10 ML LL SEM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -5520,7 +5524,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>22080452</t>
+          <t>1132410</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
@@ -5542,16 +5546,16 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>4691</v>
+        <v>4991</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>10030079</t>
+          <t>10030075</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>TOUCA DESCARTAVEL</t>
+          <t>SERINGA 5 ML LL SEM TRAVA DE SEGURANCA</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -5561,7 +5565,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>210310000</t>
+          <t>1048024</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -5583,129 +5587,140 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>4820</v>
+        <v>5024</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
+          <t>10030078</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>SWAB ALCOOL 70°</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>23020106</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>5020</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>10030078</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>SWAB ALCOOL 70°</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>22080452</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>5013</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>10030079</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>TOUCA DESCARTAVEL</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>210310000</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>5144</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
           <t>10030083</t>
         </is>
       </c>
-      <c r="E129" t="inlineStr">
+      <c r="E132" t="inlineStr">
         <is>
           <t xml:space="preserve">SACO DE LIXO PRETO 30L
 </t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr"/>
-      <c r="H129" t="inlineStr"/>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>UNIDADE</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>FILIAL TATUAPE-SP 1337</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>4804</v>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>10030087</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ATESTADO DE BRAVURA MES ATUAL
-</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="G130" t="inlineStr"/>
-      <c r="H130" t="inlineStr"/>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>UNIDADE</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>FILIAL TATUAPE-SP 1337</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>4805</v>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>10030096</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>ELASTICO AMARELO 500G</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="G131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>UNIDADE</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>FILIAL TATUAPE-SP 1337</t>
-        </is>
-      </c>
-      <c r="C132" t="n">
-        <v>4806</v>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>10030098</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>PAPEL SULFITE A4 75G</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -5733,16 +5748,17 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>4807</v>
+        <v>5130</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>10030099</t>
+          <t>10030087</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>BOBINA PLASTICA PICOTADA (2L)</t>
+          <t xml:space="preserve">ATESTADO DE BRAVURA MES ATUAL
+</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -5770,16 +5786,16 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>4808</v>
+        <v>5131</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>10030100</t>
+          <t>10030096</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>SACO DE LIXO PRETO 40L</t>
+          <t>ELASTICO AMARELO 500G</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -5807,16 +5823,16 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>4809</v>
+        <v>5132</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>10030102</t>
+          <t>10030098</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>SACO PLASTICO 15X22CM SEM ADESIVO</t>
+          <t>PAPEL SULFITE A4 75G</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -5844,16 +5860,16 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>4759</v>
+        <v>5133</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>10060415</t>
+          <t>10030099</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>GRAMPO 26/6 GALVANIZ 5000UN GRAMPLINE</t>
+          <t>BOBINA PLASTICA PICOTADA (2L)</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -5865,7 +5881,7 @@
       <c r="H136" t="inlineStr"/>
       <c r="I136" t="inlineStr">
         <is>
-          <t>CAIXA</t>
+          <t>UNIDADE</t>
         </is>
       </c>
     </row>
@@ -5881,16 +5897,16 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>4784</v>
+        <v>5134</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>10060419</t>
+          <t>10030100</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>ETIQ TP12 AZUL 12MM 210 ETIQ PIMACO</t>
+          <t>SACO DE LIXO PRETO 40L</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -5918,16 +5934,16 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>4785</v>
+        <v>5135</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>10060420</t>
+          <t>10030102</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>ETIQ TP12 VERMELHO 12MM 210 ETIQ PIMACO</t>
+          <t>SACO PLASTICO 15X22CM SEM ADESIVO</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -5955,16 +5971,16 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>4786</v>
+        <v>5084</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>10060439</t>
+          <t>10060415</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>COLA BASTAO 10G MAXPRINT</t>
+          <t>GRAMPO 26/6 GALVANIZ 5000UN GRAMPLINE</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -5976,7 +5992,7 @@
       <c r="H139" t="inlineStr"/>
       <c r="I139" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
+          <t>CAIXA</t>
         </is>
       </c>
     </row>
@@ -5992,16 +6008,16 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>4787</v>
+        <v>5109</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>10060441</t>
+          <t>10060419</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>LAPIS PRETO HB EVOL RED BIC</t>
+          <t>ETIQ TP12 AZUL 12MM 210 ETIQ PIMACO</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -6029,16 +6045,16 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>4788</v>
+        <v>5110</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>10060443</t>
+          <t>10060420</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>REGUA 30CM AZ POLIES 981.2 ACRIMET</t>
+          <t>ETIQ TP12 VERMELHO 12MM 210 ETIQ PIMACO</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -6066,16 +6082,16 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>4789</v>
+        <v>5112</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>10060452</t>
+          <t>10060439</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>APONTADOR C/DEP RETANG SORT C/1 CIS</t>
+          <t>COLA BASTAO 10G MAXPRINT</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -6103,16 +6119,16 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>4790</v>
+        <v>5113</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>10060456</t>
+          <t>10060441</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>CLIPS N.2/0 GALVANIZ L.LEVE 720UN</t>
+          <t>LAPIS PRETO HB EVOL RED BIC</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -6140,16 +6156,16 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>4791</v>
+        <v>5114</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>10060465</t>
+          <t>10060443</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>BORRACHA C/CAPA C/1 RADEX</t>
+          <t>REGUA 30CM AZ POLIES 981.2 ACRIMET</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -6177,16 +6193,16 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>4792</v>
+        <v>5115</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>10060467</t>
+          <t>10060452</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>CANETA ESF 1,0 VM CRISTAL BIC</t>
+          <t>APONTADOR C/DEP RETANG SORT C/1 CIS</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -6214,16 +6230,16 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>4793</v>
+        <v>5116</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>10060468</t>
+          <t>10060456</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>CANETA ESF 1.0 AZ CRISTAL BIC</t>
+          <t>CLIPS N.2/0 GALVANIZ L.LEVE 720UN</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -6251,16 +6267,16 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>4794</v>
+        <v>5117</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>10060477</t>
+          <t>10060465</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>PINCEL RETROPROJ AZ PTA 2MM PILOT</t>
+          <t>BORRACHA C/CAPA C/1 RADEX</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -6288,16 +6304,16 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>4795</v>
+        <v>5118</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>10060479</t>
+          <t>10060467</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>PINCEL RETROPROJ PT 2,00MM PILOT</t>
+          <t>CANETA ESF 1,0 VM CRISTAL BIC</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -6325,16 +6341,16 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>4796</v>
+        <v>5119</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>10060485</t>
+          <t>10060468</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>FITA DUPLA FACE PP 12X30 ADELBRAS.</t>
+          <t>CANETA ESF 1.0 AZ CRISTAL BIC</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -6362,16 +6378,16 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>4782</v>
+        <v>5120</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>10060506</t>
+          <t>10060477</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>PASTA ABA ELAST PP (MINI) CRISTAL A01B</t>
+          <t>PINCEL RETROPROJ AZ PTA 2MM PILOT</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -6399,16 +6415,16 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>4783</v>
+        <v>5121</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>10060509</t>
+          <t>10060479</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>CANETA ESF 0.8 AZ CRISTAL FINA BIC</t>
+          <t>PINCEL RETROPROJ PT 2,00MM PILOT</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -6436,16 +6452,16 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>4822</v>
+        <v>5122</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>10060534</t>
+          <t>10060485</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>ARQUIVO MORTO POLIONDA OF VERDE</t>
+          <t>FITA DUPLA FACE PP 12X30 ADELBRAS.</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -6473,16 +6489,16 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>4780</v>
+        <v>5107</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>10060557</t>
+          <t>10060506</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>PASTA L OF CR 230X335 0,15 PP</t>
+          <t>PASTA ABA ELAST PP (MINI) CRISTAL A01B</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -6510,16 +6526,16 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>4781</v>
+        <v>5108</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>10060560</t>
+          <t>10060509</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t xml:space="preserve">CADERNO 100 FOLHAS </t>
+          <t>CANETA ESF 0.8 AZ CRISTAL FINA BIC</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -6547,16 +6563,16 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>4797</v>
+        <v>5111</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>10060561</t>
+          <t>10060534</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>CANETA CORRETIVA PONTA METALICA</t>
+          <t>ARQUIVO MORTO POLIONDA OF VERDE</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -6584,16 +6600,16 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>4798</v>
+        <v>5105</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>10060574</t>
+          <t>10060557</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>FITA ADESIVA TRANSPARENTE LARGA</t>
+          <t>PASTA L OF CR 230X335 0,15 PP</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -6621,16 +6637,16 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>4799</v>
+        <v>5106</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>10060578</t>
+          <t>10060560</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>MARCA-TEXTO AMARELO</t>
+          <t xml:space="preserve">CADERNO 100 FOLHAS </t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -6658,16 +6674,16 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>4800</v>
+        <v>5123</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>10060586</t>
+          <t>10060561</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>POST-IT GRANDE</t>
+          <t>CANETA CORRETIVA PONTA METALICA</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -6695,16 +6711,16 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>4801</v>
+        <v>5124</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>10060587</t>
+          <t>10060574</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>POST-IT PEQUENO</t>
+          <t>FITA ADESIVA TRANSPARENTE LARGA</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -6732,16 +6748,16 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4810</v>
+        <v>5125</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>10061063</t>
+          <t>10060578</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>TINTA EPSON PRETA 5/ UNIVERSAL</t>
+          <t>MARCA-TEXTO AMARELO</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -6769,16 +6785,16 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4811</v>
+        <v>5126</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>10061064</t>
+          <t>10060586</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>TINTA EPSON CIANO 5/ UNIVERSAL</t>
+          <t>POST-IT GRANDE</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -6806,16 +6822,16 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>4812</v>
+        <v>5127</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>10061065</t>
+          <t>10060587</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>TINTA EPSON MAGENTA 5/ UNIVERSAL</t>
+          <t>POST-IT PEQUENO</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -6843,16 +6859,16 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>4813</v>
+        <v>5136</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>10061066</t>
+          <t>10061063</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>TINTA EPSON AMARELA 5/ UNIVERSAL</t>
+          <t>TINTA EPSON PRETA 5/ UNIVERSAL</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -6863,6 +6879,117 @@
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="inlineStr"/>
       <c r="I163" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>5137</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>10061064</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>TINTA EPSON CIANO 5/ UNIVERSAL</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr"/>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>5138</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>10061065</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>TINTA EPSON MAGENTA 5/ UNIVERSAL</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>UNIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>LAB - DESCARTÁVEIS TATUAPÉ</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>FILIAL TATUAPE-SP 1337</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>5139</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>10061066</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>TINTA EPSON AMARELA 5/ UNIVERSAL</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
+      <c r="I166" t="inlineStr">
         <is>
           <t>UNIDADE</t>
         </is>

</xml_diff>